<commit_message>
Matriz Casos Prueba V1.0
</commit_message>
<xml_diff>
--- a/02_Proyecto/06_Documentos/Matriz Casos de Prueba.xlsx
+++ b/02_Proyecto/06_Documentos/Matriz Casos de Prueba.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C43C8B-AD76-4D06-A779-2F7530022940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5231CDBE-0BE8-4174-A454-75FBBA37E0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 6" sheetId="4" r:id="rId1"/>
+    <sheet name="Hoja 1" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -115,9 +115,6 @@
     <t xml:space="preserve"> Cambio de Contraseña</t>
   </si>
   <si>
-    <t>Caso de Prueba 5: Actualizar contraseña correctamente</t>
-  </si>
-  <si>
     <t>CP-5</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>El sistema guarda la nueva contraseña y muestra un mensaje de éxito indicando que se actualizó correctamente.</t>
   </si>
   <si>
-    <t>Caso de Prueba 6: Actualizar contraseña incorrectamente</t>
-  </si>
-  <si>
     <t>CP-6</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t>Gestión de Sugerencias</t>
   </si>
   <si>
-    <t>Caso de Prueba 1: Enviar sugerencias exitosamente</t>
-  </si>
-  <si>
     <t>CP-1</t>
   </si>
   <si>
@@ -244,9 +235,6 @@
     <t>El sistema guarda la sugerencia y muestra un mensaje de éxito indicando que la sugerencia ha sido guardada correctamente.</t>
   </si>
   <si>
-    <t>Caso de Prueba 2: Intentar enviar sugerencias sin activar el check</t>
-  </si>
-  <si>
     <t>CP-2</t>
   </si>
   <si>
@@ -280,9 +268,6 @@
     <t>Actualización de Datos Personales</t>
   </si>
   <si>
-    <t>Caso de Prueba 3: Actualizar datos personales correctamente</t>
-  </si>
-  <si>
     <t>CP-3</t>
   </si>
   <si>
@@ -331,9 +316,6 @@
     <t>El sistema guarda los nuevos datos personales y muestra un mensaje de confirmación.</t>
   </si>
   <si>
-    <t>Caso de Prueba 4: Actualizar datos personales incorrectamente</t>
-  </si>
-  <si>
     <t>CP-4</t>
   </si>
   <si>
@@ -356,6 +338,24 @@
   </si>
   <si>
     <t>El sistema no guarda los cambios y muestra un mensaje de error.</t>
+  </si>
+  <si>
+    <t>Caso de Prueba 3: Actualizar contraseña correctamente</t>
+  </si>
+  <si>
+    <t>Caso de Prueba 4: Actualizar contraseña incorrectamente</t>
+  </si>
+  <si>
+    <t>Caso de Prueba 5: Enviar sugerencias exitosamente</t>
+  </si>
+  <si>
+    <t>Caso de Prueba 6: Intentar enviar sugerencias sin activar el check</t>
+  </si>
+  <si>
+    <t>Caso de Prueba 7: Actualizar datos personales correctamente</t>
+  </si>
+  <si>
+    <t>Caso de Prueba 8: Actualizar datos personales incorrectamente</t>
   </si>
 </sst>
 </file>
@@ -557,10 +557,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1174,8 +1174,8 @@
   </sheetPr>
   <dimension ref="A5:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1195,14 +1195,14 @@
       <c r="A6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="13"/>
     </row>
     <row r="7" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -1299,7 +1299,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3"/>
     </row>
@@ -1389,16 +1389,16 @@
     </row>
     <row r="29" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="12"/>
+        <v>106</v>
+      </c>
+      <c r="B29" s="13"/>
     </row>
     <row r="30" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="C30" s="3"/>
     </row>
@@ -1407,7 +1407,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="6"/>
     </row>
@@ -1425,7 +1425,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="6"/>
     </row>
@@ -1434,7 +1434,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" s="6"/>
     </row>
@@ -1478,61 +1478,61 @@
     </row>
     <row r="39" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="C39" s="16"/>
     </row>
     <row r="40" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C40" s="16"/>
     </row>
     <row r="41" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="C41" s="16"/>
     </row>
     <row r="42" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C42" s="16"/>
     </row>
     <row r="43" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C43" s="17"/>
     </row>
     <row r="44" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="12"/>
+        <v>107</v>
+      </c>
+      <c r="B44" s="13"/>
     </row>
     <row r="45" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="C45" s="3"/>
     </row>
@@ -1541,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C46" s="6"/>
     </row>
@@ -1550,7 +1550,7 @@
         <v>6</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C47" s="6"/>
     </row>
@@ -1559,7 +1559,7 @@
         <v>8</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C48" s="6"/>
     </row>
@@ -1568,7 +1568,7 @@
         <v>10</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C49" s="6"/>
     </row>
@@ -1612,67 +1612,67 @@
     </row>
     <row r="54" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="C54" s="16"/>
     </row>
     <row r="55" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C55" s="16"/>
     </row>
     <row r="56" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56" s="16"/>
     </row>
     <row r="57" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C57" s="16"/>
     </row>
     <row r="58" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C58" s="17"/>
     </row>
     <row r="59" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" s="12"/>
+      <c r="A59" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="13"/>
     </row>
     <row r="60" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="B60" s="13"/>
     </row>
     <row r="61" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C61" s="3"/>
     </row>
@@ -1681,7 +1681,7 @@
         <v>4</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C62" s="6"/>
     </row>
@@ -1699,7 +1699,7 @@
         <v>8</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C64" s="6"/>
     </row>
@@ -1708,7 +1708,7 @@
         <v>10</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C65" s="6"/>
     </row>
@@ -1746,76 +1746,76 @@
         <v>18</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C69" s="16"/>
     </row>
     <row r="70" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C70" s="16"/>
     </row>
     <row r="71" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C71" s="16"/>
     </row>
     <row r="72" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C72" s="16"/>
     </row>
     <row r="73" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C73" s="16"/>
     </row>
     <row r="74" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C74" s="16"/>
     </row>
     <row r="75" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C75" s="17"/>
     </row>
     <row r="76" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B76" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="B76" s="13"/>
     </row>
     <row r="77" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C77" s="3"/>
     </row>
@@ -1824,7 +1824,7 @@
         <v>4</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C78" s="6"/>
     </row>
@@ -1833,7 +1833,7 @@
         <v>6</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C79" s="6"/>
     </row>
@@ -1842,7 +1842,7 @@
         <v>8</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C80" s="6"/>
     </row>
@@ -1851,7 +1851,7 @@
         <v>10</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C81" s="6"/>
     </row>
@@ -1889,82 +1889,82 @@
         <v>18</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C85" s="16"/>
     </row>
     <row r="86" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C86" s="16"/>
     </row>
     <row r="87" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C87" s="16"/>
     </row>
     <row r="88" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C88" s="16"/>
     </row>
     <row r="89" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C89" s="16"/>
     </row>
     <row r="90" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C90" s="16"/>
     </row>
     <row r="91" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C91" s="17"/>
     </row>
     <row r="92" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B92" s="12"/>
+      <c r="A92" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" s="13"/>
     </row>
     <row r="93" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B93" s="12"/>
+        <v>110</v>
+      </c>
+      <c r="B93" s="13"/>
     </row>
     <row r="94" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="C94" s="3"/>
     </row>
@@ -1973,7 +1973,7 @@
         <v>4</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C95" s="6"/>
     </row>
@@ -1991,7 +1991,7 @@
         <v>8</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C97" s="6"/>
     </row>
@@ -2000,7 +2000,7 @@
         <v>10</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C98" s="6"/>
     </row>
@@ -2035,70 +2035,70 @@
     </row>
     <row r="102" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C102" s="16"/>
     </row>
     <row r="103" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C103" s="16"/>
     </row>
     <row r="104" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C104" s="16"/>
     </row>
     <row r="105" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C105" s="16"/>
     </row>
     <row r="106" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C106" s="16"/>
     </row>
     <row r="107" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C107" s="17"/>
     </row>
     <row r="108" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B108" s="12"/>
+        <v>111</v>
+      </c>
+      <c r="B108" s="13"/>
     </row>
     <row r="109" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="C109" s="9"/>
     </row>
@@ -2107,7 +2107,7 @@
         <v>4</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C110" s="11"/>
     </row>
@@ -2116,7 +2116,7 @@
         <v>6</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C111" s="6"/>
     </row>
@@ -2125,7 +2125,7 @@
         <v>8</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C112" s="6"/>
     </row>
@@ -2134,7 +2134,7 @@
         <v>10</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C113" s="6"/>
     </row>
@@ -2169,55 +2169,55 @@
     </row>
     <row r="117" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C117" s="16"/>
     </row>
     <row r="118" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C118" s="16"/>
     </row>
     <row r="119" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C119" s="16"/>
     </row>
     <row r="120" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C120" s="16"/>
     </row>
     <row r="121" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C121" s="16"/>
     </row>
     <row r="122" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C122" s="17"/>
     </row>

</xml_diff>